<commit_message>
minor: create website item while creating item from lead item
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lead Items" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -29,6 +29,12 @@
     <t xml:space="preserve">Photo</t>
   </si>
   <si>
+    <t xml:space="preserve">Item Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Disabled</t>
   </si>
   <si>
@@ -119,13 +125,19 @@
     <t xml:space="preserve">item_photo</t>
   </si>
   <si>
-    <t xml:space="preserve">disabled</t>
+    <t xml:space="preserve">item_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_disabled</t>
   </si>
   <si>
     <t xml:space="preserve">is_quoted</t>
   </si>
   <si>
-    <t xml:space="preserve">sample_validated</t>
+    <t xml:space="preserve">is_sample_validated</t>
   </si>
   <si>
     <t xml:space="preserve">is_po_created</t>
@@ -173,7 +185,7 @@
     <t xml:space="preserve">racking_bag</t>
   </si>
   <si>
-    <t xml:space="preserve">moq</t>
+    <t xml:space="preserve">minimum_order_qty</t>
   </si>
   <si>
     <t xml:space="preserve">unit_price</t>
@@ -453,36 +465,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="23.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="24" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="26" style="0" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -566,6 +578,12 @@
       </c>
       <c r="AA1" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -584,13 +602,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO28"/>
+  <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.45"/>
@@ -599,13 +617,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1</v>
@@ -624,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -633,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -642,7 +660,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -651,40 +669,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="7"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="8"/>
-      <c r="AL6" s="8"/>
-      <c r="AM6" s="8"/>
-      <c r="AN6" s="8"/>
-      <c r="AO6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -693,16 +687,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -711,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -720,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -729,7 +747,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -738,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -747,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -756,7 +774,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -765,7 +783,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -774,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -783,7 +801,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -792,7 +810,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -801,7 +819,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -810,7 +828,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -819,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -828,7 +846,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -837,7 +855,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -846,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" s="5"/>
     </row>
@@ -855,7 +873,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -864,7 +882,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -872,10 +890,28 @@
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>56</v>
+      <c r="B28" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
minor: remove port of loading in excel template
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lead Items" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -107,9 +107,6 @@
     <t xml:space="preserve">Certificates Required</t>
   </si>
   <si>
-    <t xml:space="preserve">Port Of Loading</t>
-  </si>
-  <si>
     <t xml:space="preserve">HEADER</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve">is_certificates_reqd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">port_of_loading</t>
   </si>
 </sst>
 </file>
@@ -465,13 +459,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -494,7 +488,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="26" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="26" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -581,9 +576,6 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -602,10 +594,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO30"/>
+  <dimension ref="A1:AO29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -617,13 +609,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1</v>
@@ -642,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -651,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -660,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -669,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -678,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -687,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5"/>
       <c r="R8" s="6"/>
@@ -720,7 +712,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -729,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -738,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -747,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="5"/>
     </row>
@@ -756,7 +748,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -765,7 +757,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -774,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -783,7 +775,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -792,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -801,7 +793,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5"/>
     </row>
@@ -810,7 +802,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5"/>
     </row>
@@ -819,7 +811,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -828,7 +820,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -837,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -846,7 +838,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -855,7 +847,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5"/>
     </row>
@@ -864,7 +856,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5"/>
     </row>
@@ -873,7 +865,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="5"/>
     </row>
@@ -882,7 +874,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="5"/>
     </row>
@@ -891,7 +883,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -900,18 +892,9 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix: add princing rule columns in quotation excel
is_abandoned removed in Lead Item
is_item_created added in Lead Item
set item price uom = item stock uom while creating items from Lead item
set pq_perc in photo quotation
on submit of po create email attachment files
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t xml:space="preserve">Photo</t>
   </si>
@@ -125,12 +125,13 @@
     <t xml:space="preserve">Quoted</t>
   </si>
   <si>
-    <t xml:space="preserve">Abandoned</t>
-  </si>
-  <si>
     <t xml:space="preserve">Samples validated</t>
   </si>
   <si>
+    <t xml:space="preserve">Item
+Created</t>
+  </si>
+  <si>
     <t xml:space="preserve">PO created</t>
   </si>
   <si>
@@ -272,10 +273,13 @@
     <t xml:space="preserve">is_quoted</t>
   </si>
   <si>
-    <t xml:space="preserve">is_abandoned</t>
-  </si>
-  <si>
     <t xml:space="preserve">is_sample_validated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_item_created</t>
   </si>
   <si>
     <t xml:space="preserve">is_po_created</t>
@@ -431,10 +435,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AT1048576"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ1" activeCellId="0" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -583,55 +587,6 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
@@ -650,11 +605,11 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.76"/>
@@ -956,10 +911,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,7 +922,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,7 +930,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,7 +938,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +946,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,7 +954,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,7 +962,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +970,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,7 +978,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +986,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +994,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple changes in photo quotation
set progress in pq for status
move so non sales items to discontinued table
set excel colum name expected data format
show 0 for boolen false values in excel
handle uppercase jpeg, png in item image in excel
set supplier part no in packaging excel
add delay in email dialog
</commit_message>
<xml_diff>
--- a/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
+++ b/art_collections/art_collections/doctype/photo_quotation/lead_items_art_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lead Items" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
   <si>
     <t xml:space="preserve">Photo</t>
   </si>
@@ -65,7 +65,8 @@
     <t xml:space="preserve">Packaging Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Racking bag</t>
+    <t xml:space="preserve">Racking bag
+(0 or 1)</t>
   </si>
   <si>
     <t xml:space="preserve">MOQ</t>
@@ -77,7 +78,8 @@
     <t xml:space="preserve">Selling item price (€)</t>
   </si>
   <si>
-    <t xml:space="preserve">Valid from sp</t>
+    <t xml:space="preserve">Valid from sp
+(YYYY-MM-DD)</t>
   </si>
   <si>
     <t xml:space="preserve">Volume qty</t>
@@ -86,22 +88,45 @@
     <t xml:space="preserve">Volume price</t>
   </si>
   <si>
-    <t xml:space="preserve">Valid from pr</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Valid from pr
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(YYYY-MM-DD)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Inner Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">Display box ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spécial mentions ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Certificates Required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test report</t>
+    <t xml:space="preserve">Display box ?
+(0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spécial mentions ?
+(0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificates Required ?
+(0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test report ?
+(0 or 1)</t>
   </si>
   <si>
     <t xml:space="preserve">Lead Item name</t>
@@ -150,154 +175,179 @@
     <t xml:space="preserve">Other language</t>
   </si>
   <si>
+    <t xml:space="preserve">Need photo for packaging ?
+(0 or 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packaging description excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Item #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo Quotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIELDNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKIP ROWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supplier_part_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supplier_item_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_material1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_material2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_material3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percentage3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customs_tariff_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">packing_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Racking bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">racking_bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum_order_qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid from sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_price_valid_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pricing_rule_qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pricing_rule_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid from pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pricing_rule_valid_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inner_qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display box ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_display_box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spécial mentions ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_special_mentions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificates Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_certificates_reqd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lead_item_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selling_pack_qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_disabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_quoted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_sample_validated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_item_created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_po_created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_language</t>
+  </si>
+  <si>
     <t xml:space="preserve">Need photo for packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging description excel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Item #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photo Quotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEADER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIELDNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKIP ROWS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supplier_part_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supplier_item_description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_material1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_material2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product_material3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percentage3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customs_tariff_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_thickness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">packing_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">racking_bag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minimum_order_qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit_price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_price_valid_from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pricing_rule_qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pricing_rule_price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pricing_rule_valid_from</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inner_qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_display_box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_special_mentions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_certificates_reqd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lead_item_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selling_pack_qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_quoted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_sample_validated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_item_created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_po_created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">designation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other_language</t>
   </si>
   <si>
     <t xml:space="preserve">is_need_photo_for_packaging</t>
@@ -319,7 +369,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -340,6 +390,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
     <font>
@@ -414,7 +470,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ1" activeCellId="0" sqref="AJ1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AU1" activeCellId="0" sqref="AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,7 +503,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="54.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="68.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,11 +661,11 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.76"/>
@@ -743,10 +799,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +810,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,7 +818,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,15 +826,15 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,15 +850,15 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,39 +866,39 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +906,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +914,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +922,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,7 +930,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,7 +938,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +946,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,7 +954,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,15 +962,15 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,7 +978,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,7 +986,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +994,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,7 +1002,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,7 +1010,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,15 +1018,15 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,7 +1034,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,7 +1042,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1050,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>